<commit_message>
fix bug about updating category
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -21,7 +21,7 @@
     <author>作成者</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>NO</t>
     <phoneticPr fontId="1"/>
@@ -185,6 +185,32 @@
     </rPh>
     <rPh sb="40" eb="42">
       <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>副問い合わせにLIMIT 1をつけるのを忘れていて、
+複数件返ってきていた。。。</t>
+    <rPh sb="0" eb="1">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ワス</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>フクスウ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ケン</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>カエ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -224,7 +250,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +260,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,12 +299,7 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -280,6 +307,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -584,66 +616,72 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.25" customWidth="1"/>
     <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="5">
+    <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="7">
+        <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="9">
+        <v>40507</v>
+      </c>
+      <c r="E2" s="9">
+        <v>40517</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="2">
+        <f>ROW()-1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6">
+      <c r="C3" s="2"/>
+      <c r="D3" s="3">
         <v>40516</v>
       </c>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2">
-        <v>40516</v>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
add a bug report
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>NO</t>
     <phoneticPr fontId="1"/>
@@ -211,6 +211,13 @@
     </rPh>
     <rPh sb="30" eb="31">
       <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Feedが文字化けする</t>
+    <rPh sb="5" eb="8">
+      <t>モジバ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -297,16 +304,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -616,7 +618,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -645,20 +647,20 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="7">
+      <c r="A2" s="4">
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="6">
         <v>40507</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="6">
         <v>40517</v>
       </c>
     </row>
@@ -677,11 +679,18 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="A4" s="2">
+        <f>ROW()-1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3">
+        <v>40517</v>
+      </c>
+      <c r="E4" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>